<commit_message>
listo bp, funcional e IPC
</commit_message>
<xml_diff>
--- a/www/data/diccionario_cod.variable.xlsx
+++ b/www/data/diccionario_cod.variable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facun\OneDrive\Documentos\GitHub\ceped-data\opcion-modulos-paneles\www\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Guido\Trabajo\Repositorios de R\Repos Propios\ceped-data\www\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB9DCD2-B0FF-4672-A2E0-1CD3CFDF1985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164A5FB9-D729-4D6F-A025-F613305FF67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -515,9 +515,6 @@
     <t>Desconocidos</t>
   </si>
   <si>
-    <t>Esta variable indica la evolución anual del Índice de Precios al Consumidor (2017 = 100). La fuente de los datos presentados corresponde en primer lugar a la información publicada por INDEC para GBA hasta 2007. Luego, al índice elaborado por CIFRA, a partir de la evolución del IPC de órganos de estadística provinciales no intervenidos hasta abril de 2016. A partir de entonces se presentan los datos elaborados por INDEC para GBA hasta diciembre de 2016, momento en el cual se toma la información de cobertura nacional publicada por el mismo organismo.</t>
-  </si>
-  <si>
     <t>Esta variable indica la evolución mensual del Índice de Precios al Consumidor (Enero 2006 = 100). La fuente de los datos presentados corresponde en primer lugar a la información publicada por INDEC para GBA hasta 2007. Luego, al índice elaborado por CIFRA, a partir de la evolución del IPC de órganos de estadística provinciales no intervenidos hasta abril de 2016. A partir de entonces se presentan los datos elaborados por INDEC para GBA hasta diciembre de 2016, momento en el cual se toma la información de cobertura nacional publicada por el mismo organismo.</t>
   </si>
   <si>
@@ -525,6 +522,9 @@
   </si>
   <si>
     <t>Esta variable indica la evolución anual del Índices de Precios al Consumidor (2017 = 100). Se han promediado los valores mensuales para facilitar su uso para deflactar los datos de ingresos de la EPH. La fuente de los datos presentados corresponde en primer lugar a la información publicada por INDEC para GBA hasta 2007. Luego, al índice elaborado por CIFRA, a partir de la evolución del IPC de órganos de estadística provinciales no intervenidos hasta abril de 2016. A partir de entonces se presentan los datos elaborados por INDEC para GBA hasta diciembre de 2016, momento en el cual se toma la información de cobertura nacional publicada por el mismo organismo.</t>
+  </si>
+  <si>
+    <t>Esta variable indica la evolución anual del Índice de Precios al Consumidor (2017 = 100). El valor anual del índice surge de un promedio de los índices mensuales, de allí que la varición anual calculada no se corresponde con la variación interanual de algún mes específico. La fuente de los datos presentados corresponde en primer lugar a la información publicada por INDEC para GBA hasta 2007. Luego, al índice elaborado por CIFRA, a partir de la evolución del IPC de órganos de estadística provinciales no intervenidos hasta abril de 2016. A partir de entonces se presentan los datos elaborados por INDEC para GBA hasta diciembre de 2016, momento en el cual se toma la información de cobertura nacional publicada por el mismo organismo.</t>
   </si>
 </sst>
 </file>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,7 +1628,7 @@
         <v>93</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1642,7 +1642,7 @@
         <v>93</v>
       </c>
       <c r="D64" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1656,7 +1656,7 @@
         <v>93</v>
       </c>
       <c r="D65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1670,7 +1670,7 @@
         <v>93</v>
       </c>
       <c r="D66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>